<commit_message>
fix bug and add blogs and pages
</commit_message>
<xml_diff>
--- a/OSM/wwwroot/export-files/Bill_4.xlsx
+++ b/OSM/wwwroot/export-files/Bill_4.xlsx
@@ -7,16 +7,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
-    <sheet name="TEDUOrder" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="OSM Order" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" iterateDelta="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>OSM</t>
   </si>
@@ -31,13 +29,13 @@
     <t>Saler Phone:</t>
   </si>
   <si>
-    <t>Customer Name: bill 1</t>
-  </si>
-  <si>
-    <t>Address: add bill 1</t>
-  </si>
-  <si>
-    <t>Phone: 1234</t>
+    <t>Customer Name: User 1</t>
+  </si>
+  <si>
+    <t>Address: 228/21 abc, xyz</t>
+  </si>
+  <si>
+    <t>Phone: 12312321312</t>
   </si>
   <si>
     <t>TT</t>
@@ -58,16 +56,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Product 10</t>
-  </si>
-  <si>
-    <t>2342342</t>
-  </si>
-  <si>
-    <t>1,000</t>
-  </si>
-  <si>
-    <t>2,342,342,000</t>
+    <t>Toy 7</t>
+  </si>
+  <si>
+    <t>150,000</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -76,7 +68,7 @@
     <t xml:space="preserve">Total amount (by word):   dong</t>
   </si>
   <si>
-    <t>1, 1, 1</t>
+    <t>15, 5, 2019</t>
   </si>
   <si>
     <t>CUSTOMER</t>
@@ -281,6 +273,9 @@
     <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -293,6 +288,9 @@
     <xf numFmtId="165" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -310,12 +308,6 @@
     </xf>
     <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -600,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -614,33 +606,33 @@
   </cols>
   <sheetData>
     <row r="1" ht="67.5" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="26"/>
     </row>
     <row r="4" ht="20.1" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="18"/>
@@ -691,13 +683,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>15</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" ht="18" customHeight="1">
@@ -869,22 +861,22 @@
       </c>
     </row>
     <row r="24" ht="18" customHeight="1">
-      <c r="A24" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="25"/>
+      <c r="A24" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="27"/>
       <c r="C24" s="4">
         <f>SUM(C9:C23)</f>
         <v>0</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" ht="30.75" customHeight="1">
+      <c r="A26" s="28" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="26" ht="30.75" customHeight="1">
-      <c r="A26" s="26" t="s">
-        <v>18</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
@@ -892,22 +884,22 @@
       <c r="E26" s="19"/>
     </row>
     <row r="28">
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -928,30 +920,4 @@
   <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>